<commit_message>
Moved the gui.py to the Nuk folder. Added screens for the gui and made the inital Appliaction system.
</commit_message>
<xml_diff>
--- a/Nuk/List of commands from Nuk.xlsx
+++ b/Nuk/List of commands from Nuk.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bragebartnes/DEV/VSCode/PhD-stuff/ME310/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bragebartnes/DEV/VSCode/PhD-stuff/ME310/ME310/Nuk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F896EA-4411-FE46-9D72-6973F9799DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18B593E-F150-AD40-B8C2-0A66062715B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{44CE020C-6734-F544-A45A-4405BF041B0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
   <si>
     <t>ACTION</t>
   </si>
@@ -122,9 +122,6 @@
     <t>EXTRUDE</t>
   </si>
   <si>
-    <t>Expexted respins OpenRB</t>
-  </si>
-  <si>
     <t>Expexted response MEGA</t>
   </si>
   <si>
@@ -204,6 +201,21 @@
   </si>
   <si>
     <t>(De)Actiavtes suction and moves gantry</t>
+  </si>
+  <si>
+    <t>Remove cartridge</t>
+  </si>
+  <si>
+    <t>REMOVECTRG</t>
+  </si>
+  <si>
+    <t>Expexted response OpenRB</t>
+  </si>
+  <si>
+    <t>CTRG RDY</t>
+  </si>
+  <si>
+    <t>Lifts all the pinions</t>
   </si>
 </sst>
 </file>
@@ -681,7 +693,7 @@
     <tableColumn id="1" xr3:uid="{1866B2BC-A099-E94F-965F-ECB79C8C9120}" name="ACTION" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{E0F9B4F8-C503-1549-987B-EE1652D1F0B8}" name="COMMAND &quot;argument&quot;" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{8D2BAA53-B65D-E244-BCE3-5D294A3D83BD}" name="ARGUMENT" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6FBF96B9-A0F4-C84F-A193-09FAF574EEB4}" name="Expexted respins OpenRB" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6FBF96B9-A0F4-C84F-A193-09FAF574EEB4}" name="Expexted response OpenRB" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{FADB9C39-874C-094D-837E-74755E25349C}" name="Expexted response MEGA" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{EA7C96E7-136E-0940-824D-D3C4B1016789}" name="Comment" dataDxfId="0"/>
   </tableColumns>
@@ -1008,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5D5AFD-C3AF-FB43-A221-D4D6ED886F90}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -1050,13 +1062,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="F2" s="13"/>
     </row>
@@ -1071,10 +1083,10 @@
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -1089,10 +1101,10 @@
         <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="8"/>
     </row>
@@ -1107,10 +1119,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -1125,10 +1137,10 @@
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -1143,16 +1155,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" ht="22" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>20</v>
@@ -1161,13 +1173,13 @@
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="22" x14ac:dyDescent="0.3">
@@ -1179,13 +1191,13 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="22" x14ac:dyDescent="0.3">
@@ -1197,13 +1209,13 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="F10" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="22" x14ac:dyDescent="0.3">
@@ -1215,58 +1227,66 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="22" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="14" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="22" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Addition of the second OpenRB
</commit_message>
<xml_diff>
--- a/Nuk/List of commands from Nuk.xlsx
+++ b/Nuk/List of commands from Nuk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bragebartnes/DEV/VSCode/PhD-stuff/ME310/ME310/Nuk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83680426-8D81-F649-81EA-11AA2CF943D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7D8A7-5315-B142-A0EF-E3936277EB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{44CE020C-6734-F544-A45A-4405BF041B0A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{44CE020C-6734-F544-A45A-4405BF041B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>ACTION</t>
   </si>
@@ -44,9 +44,6 @@
     <t>ARGUMENT</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Mover arm</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>LIFT "position" "dir"</t>
   </si>
   <si>
-    <t>NORMAL/BLOOD/CHOCOLAT/STRG; UP/DOWN</t>
-  </si>
-  <si>
     <t>Grab Petridish</t>
   </si>
   <si>
@@ -131,9 +125,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>LIFT UP / LIFT DOWN</t>
-  </si>
-  <si>
     <t>RELEASED</t>
   </si>
   <si>
@@ -173,18 +164,6 @@
     <t>PREP START -&gt; FILAMENT RDY</t>
   </si>
   <si>
-    <t>Get dish</t>
-  </si>
-  <si>
-    <t>GET "position"</t>
-  </si>
-  <si>
-    <t>DISH RDY</t>
-  </si>
-  <si>
-    <t>Combination of seveal functions. When called it should fetch a dish from selected area.</t>
-  </si>
-  <si>
     <t>NORMAL/BLOOD/CHOCOLAT/STRG/WORK AREA</t>
   </si>
   <si>
@@ -209,13 +188,28 @@
     <t>REMOVECTRG</t>
   </si>
   <si>
-    <t>Expexted response OpenRB</t>
-  </si>
-  <si>
     <t>CTRG RDY</t>
   </si>
   <si>
     <t>Lifts all the pinions</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>Expexted response OpenRB1</t>
+  </si>
+  <si>
+    <t>Expexted result OpenRB2</t>
+  </si>
+  <si>
+    <t>UP-&gt; top (right below petri), DOWN-&gt; Bottom, MID-&gt; 1 Petri heigh lower than UP, TOP-&gt; 1 Petri higher than UP</t>
+  </si>
+  <si>
+    <t>LIFT UP / LIFT DOWN /LIFT MID /LIFT TOP</t>
+  </si>
+  <si>
+    <t>NORMAL/BLOOD/CHOCOLAT/STRG; UP/DOWN/MID/TOP</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -687,15 +715,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44FF03C1-F422-9047-8B02-2650F2823225}" name="Tabell1" displayName="Tabell1" ref="A1:F25" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F25" xr:uid="{44FF03C1-F422-9047-8B02-2650F2823225}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1866B2BC-A099-E94F-965F-ECB79C8C9120}" name="ACTION" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{E0F9B4F8-C503-1549-987B-EE1652D1F0B8}" name="COMMAND &quot;argument&quot;" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8D2BAA53-B65D-E244-BCE3-5D294A3D83BD}" name="ARGUMENT" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{6FBF96B9-A0F4-C84F-A193-09FAF574EEB4}" name="Expexted response OpenRB" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{FADB9C39-874C-094D-837E-74755E25349C}" name="Expexted response MEGA" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{EA7C96E7-136E-0940-824D-D3C4B1016789}" name="Comment" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44FF03C1-F422-9047-8B02-2650F2823225}" name="Tabell1" displayName="Tabell1" ref="A1:G24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:G24" xr:uid="{44FF03C1-F422-9047-8B02-2650F2823225}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{1866B2BC-A099-E94F-965F-ECB79C8C9120}" name="ACTION" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{E0F9B4F8-C503-1549-987B-EE1652D1F0B8}" name="COMMAND &quot;argument&quot;" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8D2BAA53-B65D-E244-BCE3-5D294A3D83BD}" name="ARGUMENT" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{6FBF96B9-A0F4-C84F-A193-09FAF574EEB4}" name="Expexted response OpenRB1" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FADB9C39-874C-094D-837E-74755E25349C}" name="Expexted response MEGA" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{EA7C96E7-136E-0940-824D-D3C4B1016789}" name="Expexted result OpenRB2" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{80A8B76C-D582-7745-962A-2CD53EC22BB0}" name="COMMENT" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1018,363 +1047,376 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5D5AFD-C3AF-FB43-A221-D4D6ED886F90}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
-    <col min="3" max="3" width="57.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="97.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="102.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>6</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>56</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="D14" s="8"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
       <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
       <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="9"/>
       <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
       <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
       <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
       <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" ht="22" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="11"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="22" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hopefully got everyting now
</commit_message>
<xml_diff>
--- a/Nuk/List of commands from Nuk.xlsx
+++ b/Nuk/List of commands from Nuk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bragebartnes/DEV/VSCode/PhD-stuff/ME310/ME310/Nuk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7D8A7-5315-B142-A0EF-E3936277EB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E5D94-537E-4F4E-B75D-576166BFF874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{44CE020C-6734-F544-A45A-4405BF041B0A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{44CE020C-6734-F544-A45A-4405BF041B0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>ACTION</t>
   </si>
@@ -182,18 +182,6 @@
     <t>(De)Actiavtes suction and moves gantry</t>
   </si>
   <si>
-    <t>Remove cartridge</t>
-  </si>
-  <si>
-    <t>REMOVECTRG</t>
-  </si>
-  <si>
-    <t>CTRG RDY</t>
-  </si>
-  <si>
-    <t>Lifts all the pinions</t>
-  </si>
-  <si>
     <t>COMMENT</t>
   </si>
   <si>
@@ -210,6 +198,39 @@
   </si>
   <si>
     <t>NORMAL/BLOOD/CHOCOLAT/STRG; UP/DOWN/MID/TOP</t>
+  </si>
+  <si>
+    <t>Lift all</t>
+  </si>
+  <si>
+    <t>LIFT ALL "dir"</t>
+  </si>
+  <si>
+    <t>UP/DOWN/MID/TOP</t>
+  </si>
+  <si>
+    <t>Lifts all the "cartige" at the same time to the hight level given by "dir"</t>
+  </si>
+  <si>
+    <t>ALL LIFT UP /ALL LIFT DOWN /ALL LIFT MID /ALL LIFT TOP</t>
+  </si>
+  <si>
+    <t>Grab all</t>
+  </si>
+  <si>
+    <t>Releas all</t>
+  </si>
+  <si>
+    <t>GRAB ALL</t>
+  </si>
+  <si>
+    <t>RELEASE ALL</t>
+  </si>
+  <si>
+    <t>RELEASED ALL</t>
+  </si>
+  <si>
+    <t>GRABBED ALL</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5D5AFD-C3AF-FB43-A221-D4D6ED886F90}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1058,7 +1079,7 @@
     <col min="1" max="1" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.5" customWidth="1"/>
     <col min="3" max="3" width="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="102.5" bestFit="1" customWidth="1"/>
@@ -1075,16 +1096,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="22" x14ac:dyDescent="0.3">
@@ -1103,7 +1124,9 @@
       <c r="E2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="13"/>
+      <c r="F2" s="13" t="s">
+        <v>28</v>
+      </c>
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" ht="22" x14ac:dyDescent="0.3">
@@ -1114,17 +1137,19 @@
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G3" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22" x14ac:dyDescent="0.3">
@@ -1185,7 +1210,9 @@
       <c r="E6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="22" x14ac:dyDescent="0.3">
@@ -1204,7 +1231,9 @@
       <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="22" x14ac:dyDescent="0.3">
@@ -1223,7 +1252,9 @@
       <c r="E8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G8" s="8" t="s">
         <v>47</v>
       </c>
@@ -1235,14 +1266,18 @@
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G9" s="8" t="s">
         <v>43</v>
       </c>
@@ -1254,14 +1289,18 @@
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G10" s="8" t="s">
         <v>44</v>
       </c>
@@ -1273,14 +1312,18 @@
       <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G11" s="8" t="s">
         <v>45</v>
       </c>
@@ -1292,49 +1335,83 @@
       <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D12" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" ht="22" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="8"/>
+        <v>55</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="D13" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="G13" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="22" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
+      <c r="A14" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="22" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:7" ht="22" x14ac:dyDescent="0.3">

</xml_diff>